<commit_message>
Caso de prueba 3 actualizado
</commit_message>
<xml_diff>
--- a/Test_cases/_caso de prueba 3.xlsx
+++ b/Test_cases/_caso de prueba 3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lautaroacosta/Documents/Facultad/Testing/Grupo0102/Test_cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moren\Documents\GitHub\Grupo0102\Test_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003E6338-0416-9E47-8AD4-00881C742C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77440A9-7B66-4018-899C-4CF7A4EFC6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="500" windowWidth="28460" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="80">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -31,9 +31,6 @@
     <t>Test Case Description</t>
   </si>
   <si>
-    <t>Usuario modifica la cuenta</t>
-  </si>
-  <si>
     <t>Created By</t>
   </si>
   <si>
@@ -224,13 +221,52 @@
   </si>
   <si>
     <t>User modificate account  (Principal Scenario)</t>
+  </si>
+  <si>
+    <t>User modifies account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User signs in with new password to verify changes </t>
+  </si>
+  <si>
+    <t>Sign in succesfully</t>
+  </si>
+  <si>
+    <t>User signs in with new email to verify changes</t>
+  </si>
+  <si>
+    <t>Signs in succesfully</t>
+  </si>
+  <si>
+    <t>Enter new id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enter new email </t>
+  </si>
+  <si>
+    <t>User try to change his name (Alternative Scenario)</t>
+  </si>
+  <si>
+    <t>Enter new name</t>
+  </si>
+  <si>
+    <t>Name should be verified</t>
+  </si>
+  <si>
+    <t>User checks profile to verify changes</t>
+  </si>
+  <si>
+    <t>New name should appear</t>
+  </si>
+  <si>
+    <t>New id should appear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -345,18 +381,31 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -711,7 +760,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -738,68 +786,23 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -808,8 +811,54 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1028,20 +1077,21 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:O81"/>
+  <dimension ref="A1:O80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1051,12 +1101,12 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="82" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="83"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="D1" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="57"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
@@ -1066,22 +1116,22 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
     </row>
-    <row r="2" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" s="8"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
@@ -1091,16 +1141,16 @@
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
     </row>
-    <row r="3" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>9</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="12">
         <v>2.1</v>
@@ -1116,7 +1166,7 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="4"/>
@@ -1133,19 +1183,19 @@
       <c r="N4" s="13"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>11</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -1158,7 +1208,7 @@
       <c r="N5" s="13"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="18"/>
@@ -1166,10 +1216,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
+        <v>14</v>
+      </c>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
@@ -1179,22 +1229,22 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="19">
         <v>2</v>
       </c>
       <c r="E7" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
+        <v>16</v>
+      </c>
+      <c r="F7" s="50"/>
+      <c r="G7" s="50"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
@@ -1204,22 +1254,22 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="19">
         <v>1</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="19">
         <v>3</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
+        <v>18</v>
+      </c>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -1229,22 +1279,22 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="23">
         <v>2</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="19">
         <v>4</v>
       </c>
       <c r="E9" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="58"/>
-      <c r="G9" s="58"/>
+        <v>20</v>
+      </c>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -1254,7 +1304,7 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
     </row>
-    <row r="10" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="26"/>
       <c r="B10" s="27"/>
       <c r="C10" s="4"/>
@@ -1262,10 +1312,10 @@
         <v>5</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="58"/>
-      <c r="G10" s="58"/>
+        <v>21</v>
+      </c>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -1275,7 +1325,7 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
     </row>
-    <row r="11" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="26"/>
       <c r="B11" s="27"/>
       <c r="C11" s="4"/>
@@ -1283,7 +1333,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="13"/>
       <c r="G11" s="4"/>
@@ -1296,7 +1346,7 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="4"/>
@@ -1304,10 +1354,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
+        <v>23</v>
+      </c>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
@@ -1317,15 +1367,15 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="13"/>
-      <c r="B13" s="4"/>
+      <c r="B13" s="83"/>
       <c r="C13" s="4"/>
       <c r="D13" s="19">
         <v>8</v>
       </c>
       <c r="E13" s="28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F13" s="13"/>
       <c r="G13" s="29"/>
@@ -1338,7 +1388,7 @@
       <c r="N13" s="29"/>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1346,22 +1396,22 @@
         <v>9</v>
       </c>
       <c r="E14" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="31"/>
+      <c r="G14" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="31"/>
-      <c r="G14" s="78" t="s">
-        <v>27</v>
-      </c>
-      <c r="H14" s="79"/>
-      <c r="I14" s="79"/>
-      <c r="J14" s="79"/>
-      <c r="K14" s="79"/>
-      <c r="L14" s="79"/>
-      <c r="M14" s="79"/>
-      <c r="N14" s="80"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="60"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1369,53 +1419,53 @@
         <v>10</v>
       </c>
       <c r="E15" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="31"/>
+      <c r="G15" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="31"/>
-      <c r="G15" s="81" t="s">
+      <c r="H15" s="60"/>
+      <c r="I15" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="80"/>
-      <c r="I15" s="81" t="s">
+      <c r="J15" s="60"/>
+      <c r="K15" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="80"/>
-      <c r="K15" s="81" t="s">
+      <c r="L15" s="60"/>
+      <c r="M15" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="L15" s="80"/>
-      <c r="M15" s="81" t="s">
-        <v>32</v>
-      </c>
-      <c r="N15" s="80"/>
+      <c r="N15" s="60"/>
       <c r="O15" s="4"/>
     </row>
-    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="26"/>
       <c r="E16" s="32"/>
       <c r="F16" s="31"/>
-      <c r="G16" s="81" t="s">
+      <c r="G16" s="61" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" s="60"/>
+      <c r="I16" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="H16" s="80"/>
-      <c r="I16" s="81" t="s">
+      <c r="J16" s="60"/>
+      <c r="K16" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="80"/>
-      <c r="K16" s="81" t="s">
+      <c r="L16" s="60"/>
+      <c r="M16" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="L16" s="80"/>
-      <c r="M16" s="81" t="s">
-        <v>36</v>
-      </c>
-      <c r="N16" s="80"/>
+      <c r="N16" s="60"/>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:15" ht="14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1423,62 +1473,62 @@
       <c r="E17" s="32"/>
       <c r="F17" s="33"/>
       <c r="G17" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="34" t="s">
-        <v>38</v>
-      </c>
       <c r="I17" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="J17" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="J17" s="34" t="s">
-        <v>38</v>
-      </c>
       <c r="K17" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="L17" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="L17" s="34" t="s">
-        <v>38</v>
-      </c>
       <c r="M17" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="N17" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="N17" s="35" t="s">
-        <v>38</v>
-      </c>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="26"/>
       <c r="F18" s="18"/>
       <c r="G18" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I18" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J18" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K18" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L18" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M18" s="11"/>
       <c r="N18" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O18" s="4"/>
     </row>
-    <row r="19" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1486,135 +1536,135 @@
       <c r="E19" s="8"/>
       <c r="F19" s="18"/>
       <c r="G19" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H19" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I19" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J19" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K19" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L19" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M19" s="11"/>
       <c r="N19" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A20" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="O19" s="4"/>
-    </row>
-    <row r="20" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
-      <c r="E20" s="59"/>
+      <c r="B20" s="64" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="65"/>
       <c r="F20" s="18"/>
       <c r="G20" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H20" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="L20" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="M20" s="40"/>
+      <c r="N20" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="I20" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="J20" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="K20" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="L20" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="M20" s="41"/>
-      <c r="N20" s="36" t="s">
-        <v>41</v>
-      </c>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A21" s="56"/>
-      <c r="B21" s="60"/>
-      <c r="C21" s="60"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="61"/>
+    <row r="21" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="63"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="55"/>
       <c r="F21" s="4"/>
       <c r="G21" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H21" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I21" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J21" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K21" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L21" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M21" s="11"/>
       <c r="N21" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="42" t="s">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="44" t="s">
+      <c r="E22" s="44" t="s">
         <v>45</v>
-      </c>
-      <c r="E22" s="45" t="s">
-        <v>46</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H22" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I22" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J22" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K22" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L22" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M22" s="11"/>
       <c r="N22" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1622,326 +1672,337 @@
       <c r="E23" s="8"/>
       <c r="F23" s="4"/>
       <c r="G23" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H23" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="L23" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="M23" s="40"/>
+      <c r="N23" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="J23" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="K23" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="L23" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="M23" s="41"/>
-      <c r="N23" s="36" t="s">
-        <v>41</v>
-      </c>
       <c r="O23" s="4"/>
     </row>
-    <row r="24" spans="1:15" ht="14" x14ac:dyDescent="0.2">
-      <c r="A24" s="46" t="s">
+    <row r="24" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A24" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="62" t="s">
+      <c r="C24" s="55"/>
+      <c r="D24" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="61"/>
+      <c r="E24" s="55"/>
       <c r="F24" s="4"/>
       <c r="G24" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H24" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I24" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J24" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K24" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L24" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M24" s="11"/>
       <c r="N24" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O24" s="4"/>
     </row>
-    <row r="25" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="47">
+    <row r="25" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A25" s="46">
         <v>1</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="B25" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="52"/>
+      <c r="D25" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="65"/>
-      <c r="D25" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="65"/>
+      <c r="E25" s="52"/>
       <c r="F25" s="4"/>
       <c r="G25" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H25" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I25" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J25" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K25" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L25" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M25" s="11"/>
       <c r="N25" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A26" s="48">
+    <row r="26" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="47">
         <v>2</v>
       </c>
-      <c r="B26" s="66" t="s">
-        <v>52</v>
-      </c>
-      <c r="C26" s="61"/>
-      <c r="D26" s="66" t="s">
+      <c r="B26" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E26" s="61"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" s="55"/>
       <c r="F26" s="4"/>
       <c r="G26" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H26" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="L26" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="M26" s="40"/>
+      <c r="N26" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="I26" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="J26" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="K26" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="L26" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="M26" s="41"/>
-      <c r="N26" s="36" t="s">
-        <v>41</v>
-      </c>
       <c r="O26" s="4"/>
     </row>
-    <row r="27" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A27" s="47">
+    <row r="27" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A27" s="46">
         <v>3</v>
       </c>
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="55"/>
+      <c r="D27" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="E27" s="61"/>
+      <c r="E27" s="55"/>
       <c r="F27" s="4"/>
       <c r="G27" s="36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H27" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I27" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J27" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K27" s="37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L27" s="37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M27" s="11"/>
       <c r="N27" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A28" s="48">
+    <row r="28" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="47">
         <v>4</v>
       </c>
-      <c r="B28" s="64" t="s">
+      <c r="B28" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="52"/>
+      <c r="D28" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="65"/>
-      <c r="D28" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="E28" s="65"/>
+      <c r="E28" s="52"/>
       <c r="F28" s="4"/>
       <c r="O28" s="4"/>
     </row>
-    <row r="29" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A29" s="47">
+    <row r="29" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A29" s="46">
         <v>5</v>
       </c>
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="52"/>
+      <c r="D29" s="53" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="65"/>
-      <c r="D29" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="E29" s="65"/>
+      <c r="E29" s="52"/>
       <c r="F29" s="4"/>
       <c r="O29" s="4"/>
     </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="48">
+    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="47">
         <v>6</v>
       </c>
-      <c r="B30" s="67" t="s">
+      <c r="B30" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="52"/>
+      <c r="D30" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="65"/>
-      <c r="D30" s="67" t="s">
+      <c r="E30" s="52"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="74" t="s">
+      <c r="H30" s="52"/>
+      <c r="I30" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="J30" s="52"/>
+      <c r="K30" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="L30" s="52"/>
+      <c r="M30" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="N30" s="52"/>
+      <c r="O30" s="4"/>
+    </row>
+    <row r="31" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A31" s="77">
+        <v>7</v>
+      </c>
+      <c r="B31" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="79"/>
+      <c r="D31" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31" s="78"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="70"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="H30" s="65"/>
-      <c r="I30" s="75" t="s">
-        <v>61</v>
-      </c>
-      <c r="J30" s="65"/>
-      <c r="K30" s="75" t="s">
-        <v>61</v>
-      </c>
-      <c r="L30" s="65"/>
-      <c r="M30" s="75" t="s">
-        <v>61</v>
-      </c>
-      <c r="N30" s="65"/>
-      <c r="O30" s="4"/>
-    </row>
-    <row r="31" spans="1:15" ht="14" x14ac:dyDescent="0.2">
-      <c r="F31" s="4"/>
-      <c r="G31" s="76"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="73" t="s">
-        <v>62</v>
-      </c>
-      <c r="J31" s="61"/>
-      <c r="K31" s="77"/>
-      <c r="L31" s="61"/>
-      <c r="M31" s="71"/>
-      <c r="N31" s="61"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="72"/>
+      <c r="L31" s="55"/>
+      <c r="M31" s="73"/>
+      <c r="N31" s="55"/>
       <c r="O31" s="4"/>
     </row>
-    <row r="32" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A32" s="49"/>
-      <c r="B32" s="72"/>
-      <c r="C32" s="58"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="58"/>
+    <row r="32" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="48"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="50"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="71"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="71"/>
-      <c r="N32" s="61"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="55"/>
+      <c r="K32" s="73"/>
+      <c r="L32" s="55"/>
+      <c r="M32" s="73"/>
+      <c r="N32" s="55"/>
       <c r="O32" s="4"/>
     </row>
-    <row r="33" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A33" s="49"/>
-      <c r="B33" s="72"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="58"/>
+    <row r="33" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="48"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="50"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="70"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="71"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="71"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="71"/>
-      <c r="N33" s="61"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="52"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="55"/>
+      <c r="K33" s="73"/>
+      <c r="L33" s="55"/>
+      <c r="M33" s="73"/>
+      <c r="N33" s="55"/>
       <c r="O33" s="4"/>
     </row>
-    <row r="34" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A34" s="49"/>
-      <c r="B34" s="72"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="58"/>
+    <row r="34" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A34" s="48"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="50"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="71"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="71"/>
-      <c r="N34" s="61"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="73"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="73"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="73"/>
+      <c r="N34" s="55"/>
       <c r="O34" s="4"/>
     </row>
-    <row r="35" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A35" s="49"/>
-      <c r="B35" s="72"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="58"/>
+    <row r="35" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="48"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="50"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="71"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="71"/>
-      <c r="N35" s="61"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="73"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="73"/>
+      <c r="L35" s="55"/>
+      <c r="M35" s="73"/>
+      <c r="N35" s="55"/>
       <c r="O35" s="4"/>
     </row>
-    <row r="36" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A36" s="49"/>
-      <c r="B36" s="72"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="58"/>
+    <row r="36" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="48"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="50"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
@@ -1953,12 +2014,12 @@
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
     </row>
-    <row r="37" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A37" s="49"/>
-      <c r="B37" s="72"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="58"/>
+    <row r="37" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A37" s="48"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="50"/>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
@@ -1970,12 +2031,12 @@
       <c r="N37" s="4"/>
       <c r="O37" s="4"/>
     </row>
-    <row r="38" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A38" s="49"/>
-      <c r="B38" s="72"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="58"/>
+    <row r="38" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="48"/>
+      <c r="B38" s="49"/>
+      <c r="C38" s="50"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="50"/>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
@@ -1987,12 +2048,12 @@
       <c r="N38" s="4"/>
       <c r="O38" s="4"/>
     </row>
-    <row r="39" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A39" s="49"/>
-      <c r="B39" s="72"/>
-      <c r="C39" s="58"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="58"/>
+    <row r="39" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="48"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="50"/>
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
@@ -2004,7 +2065,7 @@
       <c r="N39" s="4"/>
       <c r="O39" s="4"/>
     </row>
-    <row r="40" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -2021,16 +2082,16 @@
       <c r="N40" s="4"/>
       <c r="O40" s="4"/>
     </row>
-    <row r="41" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A41" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="59"/>
+    <row r="41" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A41" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="65"/>
       <c r="F41" s="4"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
@@ -2042,156 +2103,156 @@
       <c r="N41" s="8"/>
       <c r="O41" s="4"/>
     </row>
-    <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="56"/>
-      <c r="B42" s="60"/>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="61"/>
+    <row r="42" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="63"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="55"/>
       <c r="F42" s="18"/>
-      <c r="G42" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="H42" s="61"/>
-      <c r="I42" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="J42" s="61"/>
-      <c r="K42" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="L42" s="61"/>
-      <c r="M42" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="N42" s="61"/>
+      <c r="G42" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="H42" s="55"/>
+      <c r="I42" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="J42" s="55"/>
+      <c r="K42" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="L42" s="55"/>
+      <c r="M42" s="76" t="s">
+        <v>60</v>
+      </c>
+      <c r="N42" s="55"/>
       <c r="O42" s="4"/>
     </row>
-    <row r="43" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="42" t="s">
+    <row r="43" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" s="11"/>
-      <c r="D43" s="44" t="s">
+      <c r="E43" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="E43" s="45" t="s">
-        <v>46</v>
-      </c>
       <c r="F43" s="4"/>
-      <c r="G43" s="68"/>
-      <c r="H43" s="61"/>
-      <c r="I43" s="73" t="s">
-        <v>64</v>
-      </c>
-      <c r="J43" s="61"/>
-      <c r="K43" s="68"/>
-      <c r="L43" s="61"/>
-      <c r="M43" s="68"/>
-      <c r="N43" s="61"/>
+      <c r="G43" s="74"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="71" t="s">
+        <v>63</v>
+      </c>
+      <c r="J43" s="55"/>
+      <c r="K43" s="74"/>
+      <c r="L43" s="55"/>
+      <c r="M43" s="74"/>
+      <c r="N43" s="55"/>
       <c r="O43" s="4"/>
     </row>
-    <row r="44" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
       <c r="F44" s="4"/>
-      <c r="G44" s="68"/>
-      <c r="H44" s="61"/>
-      <c r="I44" s="68"/>
-      <c r="J44" s="61"/>
-      <c r="K44" s="68"/>
-      <c r="L44" s="61"/>
-      <c r="M44" s="68"/>
-      <c r="N44" s="61"/>
+      <c r="G44" s="74"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="74"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="74"/>
+      <c r="L44" s="55"/>
+      <c r="M44" s="74"/>
+      <c r="N44" s="55"/>
       <c r="O44" s="4"/>
     </row>
-    <row r="45" spans="1:15" ht="14" x14ac:dyDescent="0.2">
-      <c r="A45" s="46" t="s">
+    <row r="45" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A45" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="62" t="s">
+      <c r="C45" s="55"/>
+      <c r="D45" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="61"/>
-      <c r="D45" s="62" t="s">
+      <c r="E45" s="55"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="74"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="74"/>
+      <c r="L45" s="55"/>
+      <c r="M45" s="74"/>
+      <c r="N45" s="55"/>
+      <c r="O45" s="4"/>
+    </row>
+    <row r="46" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A46" s="46">
+        <v>1</v>
+      </c>
+      <c r="B46" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="E45" s="61"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="68"/>
-      <c r="H45" s="61"/>
-      <c r="I45" s="68"/>
-      <c r="J45" s="61"/>
-      <c r="K45" s="68"/>
-      <c r="L45" s="61"/>
-      <c r="M45" s="68"/>
-      <c r="N45" s="61"/>
-      <c r="O45" s="4"/>
-    </row>
-    <row r="46" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A46" s="47">
-        <v>1</v>
-      </c>
-      <c r="B46" s="64" t="s">
+      <c r="C46" s="52"/>
+      <c r="D46" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="65"/>
-      <c r="D46" s="64" t="s">
+      <c r="E46" s="52"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="74"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="74"/>
+      <c r="J46" s="55"/>
+      <c r="K46" s="74"/>
+      <c r="L46" s="55"/>
+      <c r="M46" s="74"/>
+      <c r="N46" s="55"/>
+      <c r="O46" s="4"/>
+    </row>
+    <row r="47" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A47" s="47">
+        <v>2</v>
+      </c>
+      <c r="B47" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E46" s="65"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="68"/>
-      <c r="H46" s="61"/>
-      <c r="I46" s="68"/>
-      <c r="J46" s="61"/>
-      <c r="K46" s="68"/>
-      <c r="L46" s="61"/>
-      <c r="M46" s="68"/>
-      <c r="N46" s="61"/>
-      <c r="O46" s="4"/>
-    </row>
-    <row r="47" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A47" s="48">
-        <v>2</v>
-      </c>
-      <c r="B47" s="66" t="s">
+      <c r="C47" s="55"/>
+      <c r="D47" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" s="55"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="74"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="74"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="74"/>
+      <c r="L47" s="55"/>
+      <c r="M47" s="74"/>
+      <c r="N47" s="55"/>
+      <c r="O47" s="4"/>
+    </row>
+    <row r="48" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A48" s="46">
+        <v>3</v>
+      </c>
+      <c r="B48" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="61"/>
-      <c r="D47" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="E47" s="61"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="68"/>
-      <c r="H47" s="61"/>
-      <c r="I47" s="68"/>
-      <c r="J47" s="61"/>
-      <c r="K47" s="68"/>
-      <c r="L47" s="61"/>
-      <c r="M47" s="68"/>
-      <c r="N47" s="61"/>
-      <c r="O47" s="4"/>
-    </row>
-    <row r="48" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A48" s="47">
-        <v>3</v>
-      </c>
-      <c r="B48" s="66" t="s">
+      <c r="C48" s="55"/>
+      <c r="D48" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="61"/>
-      <c r="D48" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="E48" s="61"/>
+      <c r="E48" s="55"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
@@ -2203,18 +2264,18 @@
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
     </row>
-    <row r="49" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A49" s="48">
+    <row r="49" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A49" s="47">
         <v>4</v>
       </c>
-      <c r="B49" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="C49" s="65"/>
-      <c r="D49" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="E49" s="65"/>
+      <c r="B49" s="81" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="52"/>
+      <c r="D49" s="81" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" s="52"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
@@ -2226,18 +2287,18 @@
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
     </row>
-    <row r="50" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A50" s="47">
+    <row r="50" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="46">
         <v>5</v>
       </c>
-      <c r="B50" s="67" t="s">
+      <c r="B50" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="52"/>
+      <c r="D50" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="C50" s="65"/>
-      <c r="D50" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="E50" s="65"/>
+      <c r="E50" s="52"/>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
@@ -2249,268 +2310,356 @@
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
     </row>
-    <row r="56" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A56" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="B56" s="57" t="s">
+    <row r="51" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="80">
+        <v>6</v>
+      </c>
+      <c r="B51" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="78"/>
+      <c r="D51" s="79" t="s">
+        <v>71</v>
+      </c>
+      <c r="E51" s="78"/>
+    </row>
+    <row r="56" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A56" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="50"/>
+      <c r="D56" s="50"/>
+      <c r="E56" s="65"/>
+    </row>
+    <row r="57" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A57" s="63"/>
+      <c r="B57" s="66"/>
+      <c r="C57" s="66"/>
+      <c r="D57" s="66"/>
+      <c r="E57" s="55"/>
+    </row>
+    <row r="58" spans="1:15" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B58" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="59"/>
-    </row>
-    <row r="57" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A57" s="56"/>
-      <c r="B57" s="60"/>
-      <c r="C57" s="60"/>
-      <c r="D57" s="60"/>
-      <c r="E57" s="61"/>
-    </row>
-    <row r="58" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="42" t="s">
+      <c r="C58" s="11"/>
+      <c r="D58" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B58" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C58" s="11"/>
-      <c r="D58" s="44" t="s">
+      <c r="E58" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="E58" s="45" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" ht="13" x14ac:dyDescent="0.15">
+    </row>
+    <row r="59" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8"/>
       <c r="D59" s="8"/>
       <c r="E59" s="8"/>
     </row>
-    <row r="60" spans="1:15" ht="14" x14ac:dyDescent="0.2">
-      <c r="A60" s="46" t="s">
+    <row r="60" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A60" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B60" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="B60" s="62" t="s">
+      <c r="C60" s="55"/>
+      <c r="D60" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="C60" s="61"/>
-      <c r="D60" s="62" t="s">
+      <c r="E60" s="55"/>
+    </row>
+    <row r="61" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A61" s="46">
+        <v>1</v>
+      </c>
+      <c r="B61" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="E60" s="61"/>
-    </row>
-    <row r="61" spans="1:15" ht="13" x14ac:dyDescent="0.15">
-      <c r="A61" s="47">
-        <v>1</v>
-      </c>
-      <c r="B61" s="64" t="s">
+      <c r="C61" s="52"/>
+      <c r="D61" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="C61" s="65"/>
-      <c r="D61" s="64" t="s">
+      <c r="E61" s="52"/>
+    </row>
+    <row r="62" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A62" s="47">
+        <v>2</v>
+      </c>
+      <c r="B62" s="54" t="s">
         <v>51</v>
       </c>
-      <c r="E61" s="65"/>
-    </row>
-    <row r="62" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A62" s="48">
-        <v>2</v>
-      </c>
-      <c r="B62" s="66" t="s">
+      <c r="C62" s="55"/>
+      <c r="D62" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E62" s="55"/>
+    </row>
+    <row r="63" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A63" s="46">
+        <v>3</v>
+      </c>
+      <c r="B63" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="C62" s="61"/>
-      <c r="D62" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="E62" s="61"/>
-    </row>
-    <row r="63" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A63" s="47">
-        <v>3</v>
-      </c>
-      <c r="B63" s="66" t="s">
+      <c r="C63" s="55"/>
+      <c r="D63" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="C63" s="61"/>
-      <c r="D63" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="E63" s="61"/>
-    </row>
-    <row r="64" spans="1:15" ht="14" x14ac:dyDescent="0.15">
-      <c r="A64" s="48">
+      <c r="E63" s="55"/>
+    </row>
+    <row r="64" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A64" s="46">
         <v>4</v>
       </c>
-      <c r="B64" s="64" t="s">
-        <v>55</v>
-      </c>
-      <c r="C64" s="65"/>
-      <c r="D64" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="E64" s="65"/>
-    </row>
-    <row r="65" spans="1:5" ht="13" x14ac:dyDescent="0.15">
+      <c r="B64" s="81" t="s">
+        <v>72</v>
+      </c>
+      <c r="C64" s="52"/>
+      <c r="D64" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="E64" s="52"/>
+    </row>
+    <row r="65" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="47">
         <v>5</v>
       </c>
-      <c r="B65" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="C65" s="65"/>
-      <c r="D65" s="64" t="s">
+      <c r="B65" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="E65" s="65"/>
-    </row>
-    <row r="66" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A66" s="48">
+      <c r="C65" s="52"/>
+      <c r="D65" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="E65" s="52"/>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="80">
         <v>6</v>
       </c>
-      <c r="B66" s="67" t="s">
+      <c r="B66" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="C66" s="78"/>
+      <c r="D66" s="79" t="s">
+        <v>79</v>
+      </c>
+      <c r="E66" s="78"/>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="B69" s="82" t="s">
+        <v>74</v>
+      </c>
+      <c r="C69" s="50"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="65"/>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="63"/>
+      <c r="B70" s="66"/>
+      <c r="C70" s="66"/>
+      <c r="D70" s="66"/>
+      <c r="E70" s="55"/>
+    </row>
+    <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B71" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="C71" s="11"/>
+      <c r="D71" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E71" s="44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A73" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B73" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="C73" s="55"/>
+      <c r="D73" s="67" t="s">
+        <v>48</v>
+      </c>
+      <c r="E73" s="55"/>
+    </row>
+    <row r="74" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A74" s="46">
+        <v>1</v>
+      </c>
+      <c r="B74" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="52"/>
+      <c r="D74" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="E74" s="52"/>
+    </row>
+    <row r="75" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A75" s="47">
+        <v>2</v>
+      </c>
+      <c r="B75" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C75" s="55"/>
+      <c r="D75" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" s="55"/>
+    </row>
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="46">
+        <v>3</v>
+      </c>
+      <c r="B76" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C76" s="55"/>
+      <c r="D76" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="E76" s="55"/>
+    </row>
+    <row r="77" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A77" s="46">
+        <v>4</v>
+      </c>
+      <c r="B77" s="81" t="s">
+        <v>75</v>
+      </c>
+      <c r="C77" s="52"/>
+      <c r="D77" s="81" t="s">
+        <v>76</v>
+      </c>
+      <c r="E77" s="52"/>
+    </row>
+    <row r="78" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A78" s="47">
+        <v>5</v>
+      </c>
+      <c r="B78" s="51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C78" s="52"/>
+      <c r="D78" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="C66" s="65"/>
-      <c r="D66" s="67" t="s">
-        <v>60</v>
-      </c>
-      <c r="E66" s="65"/>
-    </row>
-    <row r="72" spans="1:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="A72" s="50"/>
-      <c r="B72" s="39"/>
-      <c r="C72" s="39"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="39"/>
-    </row>
-    <row r="73" spans="1:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="A73" s="50"/>
-      <c r="B73" s="39"/>
-      <c r="C73" s="39"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="39"/>
-    </row>
-    <row r="74" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A74" s="51"/>
-      <c r="B74" s="52"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="53"/>
-    </row>
-    <row r="75" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A75" s="4"/>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-    </row>
-    <row r="76" spans="1:5" ht="14" x14ac:dyDescent="0.2">
-      <c r="A76" s="54"/>
-      <c r="B76" s="63"/>
-      <c r="C76" s="58"/>
-      <c r="D76" s="63"/>
-      <c r="E76" s="58"/>
-    </row>
-    <row r="77" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A77" s="49"/>
-      <c r="B77" s="72"/>
-      <c r="C77" s="58"/>
-      <c r="D77" s="72"/>
-      <c r="E77" s="58"/>
-    </row>
-    <row r="78" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A78" s="49"/>
-      <c r="B78" s="72"/>
-      <c r="C78" s="58"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="58"/>
-    </row>
-    <row r="79" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A79" s="49"/>
-      <c r="B79" s="72"/>
-      <c r="C79" s="58"/>
-      <c r="D79" s="72"/>
-      <c r="E79" s="58"/>
-    </row>
-    <row r="80" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A80" s="49"/>
-      <c r="B80" s="72"/>
-      <c r="C80" s="58"/>
-      <c r="D80" s="72"/>
-      <c r="E80" s="58"/>
-    </row>
-    <row r="81" spans="1:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="A81" s="49"/>
-      <c r="B81" s="72"/>
-      <c r="C81" s="58"/>
-      <c r="D81" s="72"/>
-      <c r="E81" s="58"/>
+      <c r="E78" s="52"/>
+    </row>
+    <row r="79" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A79" s="80">
+        <v>6</v>
+      </c>
+      <c r="B79" s="79" t="s">
+        <v>77</v>
+      </c>
+      <c r="C79" s="78"/>
+      <c r="D79" s="79" t="s">
+        <v>78</v>
+      </c>
+      <c r="E79" s="78"/>
+    </row>
+    <row r="80" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A80" s="48"/>
+      <c r="B80" s="49"/>
+      <c r="C80" s="50"/>
+      <c r="D80" s="49"/>
+      <c r="E80" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="140">
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="D81:E81"/>
+  <mergeCells count="150">
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="B69:E70"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="B66:C66"/>
     <mergeCell ref="D66:E66"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="B61:C61"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="G14:N14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:E21"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="I30:J30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="I31:J31"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="M31:N31"/>
-    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="A56:A57"/>
+    <mergeCell ref="B56:E57"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="K46:L46"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="K45:L45"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="K44:L44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:E42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I34:J34"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="I35:J35"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="I42:J42"/>
+    <mergeCell ref="K42:L42"/>
+    <mergeCell ref="M42:N42"/>
     <mergeCell ref="I43:J43"/>
     <mergeCell ref="K43:L43"/>
     <mergeCell ref="M43:N43"/>
@@ -2534,65 +2683,69 @@
     <mergeCell ref="K33:L33"/>
     <mergeCell ref="M33:N33"/>
     <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="I44:J44"/>
-    <mergeCell ref="K44:L44"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B41:E42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I34:J34"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="I35:J35"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="I42:J42"/>
-    <mergeCell ref="K42:L42"/>
-    <mergeCell ref="M42:N42"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="M46:N46"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="K45:L45"/>
-    <mergeCell ref="M45:N45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="B56:E57"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:E21"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="D77:E77"/>
     <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="B61:C61"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="D79:E79"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>